<commit_message>
readying for preview preview release; notes; more
Mostly adding lots of info & references files. Sifting through loose
items to ensure playability (no errors). Basic functionality is there
for 60% of buildings and 70% of units. Art is 90% done. 3d art is 50%
done.
</commit_message>
<xml_diff>
--- a/notes/Technologies.xlsx
+++ b/notes/Technologies.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="28455" windowHeight="13425"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Technologies!$A$1:$BB$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -3065,9 +3065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A3:A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3093,7 +3093,7 @@
     <col min="55" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="5" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" s="5" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>